<commit_message>
Code cleaned and updated
</commit_message>
<xml_diff>
--- a/Data/Cinema by territorial area.xlsx
+++ b/Data/Cinema by territorial area.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertocalabrese99/Desktop/Statistical learning/Statistical_Learning_Project/Data/Cleaned data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertocalabrese99/Desktop/Statistical learning/Statistical_Learning_Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6366D0D8-00B7-C443-B898-F276D7A26B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F68295C-8BCA-224C-9925-0CA87E515960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" xr2:uid="{1F1F6805-2FDB-8F4F-9065-46E49BB6E294}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" activeTab="2" xr2:uid="{1F1F6805-2FDB-8F4F-9065-46E49BB6E294}"/>
   </bookViews>
   <sheets>
     <sheet name="Numero spettacoli" sheetId="3" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
   <si>
-    <t>Regione</t>
-  </si>
-  <si>
     <t>Liguria</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>Sicilia</t>
+  </si>
+  <si>
+    <t>Region</t>
   </si>
 </sst>
 </file>
@@ -473,15 +473,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201C2995-3A2A-3148-8866-986C366911DB}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>2018</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>97305</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>19304</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>44309</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>235480</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>260687</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>90476</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>458503</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>94582</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>542171</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>108309</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>7316</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>224096</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>184997</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>73283</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>195828</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>214259</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>32176</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>56507</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>7437</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>217665</v>
@@ -912,14 +912,14 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>2018</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>2029174</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>410093</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>946883</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>6196610</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>9451094</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>2289841</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>11783133</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>2484639</v>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>17699006</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2700195</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>157000</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>7177373</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>4825143</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1698762</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>5167763</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>6540085</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>1135408</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>1383974</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>201458</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>7410065</v>
@@ -1349,15 +1349,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5574F145-D58C-B849-A2D0-BC4F97B71DC5}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>2018</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>13776413.460000001</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>2736061.06</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>6717812.5899999999</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>41950937.600000001</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>72572539.629999995</v>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>17177559.09</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>85690578.090000004</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>18883544.800000001</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>151253801.86000001</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>18008353.100000001</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>1096311.3600000001</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>50372488.219999999</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>28737523.149999999</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>12028989.439999999</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>31225414.25</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>49183165.689999998</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>9787477.2200000007</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>10424528.789999999</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>1658434.25</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>59128819.43</v>

</xml_diff>